<commit_message>
Changes to support improved HX optimiser
</commit_message>
<xml_diff>
--- a/ESM comparison.xlsx
+++ b/ESM comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smros\OneDrive\Documents\00 CAMBRIDGE WORK\09 Thesis\Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6557C4-5C82-4128-87E8-BFD6EF908CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E06B706-7F36-4A12-8A72-277D6A9B8769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1677,7 +1677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -2146,7 +2146,7 @@
         <v>38561.200000000004</v>
       </c>
       <c r="F41">
-        <f t="shared" ref="F41:F43" si="1">1-D41/E41</f>
+        <f t="shared" ref="F41:F42" si="1">1-D41/E41</f>
         <v>0.84544049459041737</v>
       </c>
     </row>
@@ -2188,10 +2188,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8645B6D-462F-4E4A-B9DE-58950D3F6711}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2471,156 +2471,186 @@
         <v>576.82499999999993</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>58</v>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C15">
+        <f t="shared" ref="C15" si="3">1-C14/$E$14</f>
+        <v>-6.2253987984255188E-2</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ref="D15" si="4">1-D14/$E$14</f>
+        <v>-3.0142945929148457E-2</v>
+      </c>
+      <c r="E15">
+        <f>1-E14/$E$14</f>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ref="F15:I15" si="5">1-F14/$E$14</f>
+        <v>1.3258752848560151E-2</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="5"/>
+        <v>3.2193909260410103E-2</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="5"/>
+        <v>3.8367516055521023E-2</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="5"/>
+        <v>4.4002486016159192E-2</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
         <v>57</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <f>B14*0.05*121</f>
         <v>4192.6499999999996</v>
       </c>
-      <c r="C17">
-        <f t="shared" ref="C17:I17" si="3">C14*0.05*121</f>
+      <c r="C18">
+        <f t="shared" ref="C18:I18" si="6">C14*0.05*121</f>
         <v>3877.671875</v>
       </c>
-      <c r="D17">
-        <f t="shared" si="3"/>
+      <c r="D18">
+        <f t="shared" si="6"/>
         <v>3760.453125</v>
       </c>
-      <c r="E17">
-        <f t="shared" si="3"/>
+      <c r="E18">
+        <f t="shared" si="6"/>
         <v>3650.4187500000003</v>
       </c>
-      <c r="F17">
-        <f t="shared" si="3"/>
+      <c r="F18">
+        <f t="shared" si="6"/>
         <v>3602.0187500000002</v>
       </c>
-      <c r="G17">
-        <f t="shared" si="3"/>
+      <c r="G18">
+        <f t="shared" si="6"/>
         <v>3532.8975000000005</v>
       </c>
-      <c r="H17">
-        <f t="shared" si="3"/>
+      <c r="H18">
+        <f t="shared" si="6"/>
         <v>3510.3612500000004</v>
       </c>
-      <c r="I17">
-        <f t="shared" si="3"/>
+      <c r="I18">
+        <f t="shared" si="6"/>
         <v>3489.7912499999998</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
         <v>59</v>
       </c>
-      <c r="B18">
-        <f t="shared" ref="B18:I18" si="4">B13*0.05*149</f>
+      <c r="B19">
+        <f t="shared" ref="B19:I19" si="7">B13*0.05*149</f>
         <v>3742.0605</v>
       </c>
-      <c r="C18">
-        <f t="shared" si="4"/>
+      <c r="C19">
+        <f t="shared" si="7"/>
         <v>3663.6864999999998</v>
       </c>
-      <c r="D18">
-        <f t="shared" si="4"/>
+      <c r="D19">
+        <f t="shared" si="7"/>
         <v>3577.788</v>
       </c>
-      <c r="E18">
-        <f t="shared" si="4"/>
+      <c r="E19">
+        <f t="shared" si="7"/>
         <v>3487.5685000000003</v>
       </c>
-      <c r="F18">
-        <f t="shared" si="4"/>
+      <c r="F19">
+        <f t="shared" si="7"/>
         <v>3446.9659999999999</v>
       </c>
-      <c r="G18">
-        <f t="shared" si="4"/>
+      <c r="G19">
+        <f t="shared" si="7"/>
         <v>3384.3114999999998</v>
       </c>
-      <c r="H18">
-        <f t="shared" si="4"/>
+      <c r="H19">
+        <f t="shared" si="7"/>
         <v>3361.7380000000003</v>
       </c>
-      <c r="I18">
-        <f t="shared" si="4"/>
+      <c r="I19">
+        <f t="shared" si="7"/>
         <v>3341.027</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A19" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" s="1">
-        <f>B17+B18</f>
-        <v>7934.7104999999992</v>
-      </c>
-      <c r="C19" s="1">
-        <f t="shared" ref="C19:I19" si="5">C17+C18</f>
-        <v>7541.3583749999998</v>
-      </c>
-      <c r="D19" s="1">
-        <f t="shared" si="5"/>
-        <v>7338.2411250000005</v>
-      </c>
-      <c r="E19" s="1">
-        <f t="shared" si="5"/>
-        <v>7137.9872500000001</v>
-      </c>
-      <c r="F19" s="1">
-        <f t="shared" si="5"/>
-        <v>7048.9847499999996</v>
-      </c>
-      <c r="G19" s="1">
-        <f t="shared" si="5"/>
-        <v>6917.2090000000007</v>
-      </c>
-      <c r="H19" s="1">
-        <f t="shared" si="5"/>
-        <v>6872.0992500000011</v>
-      </c>
-      <c r="I19" s="1">
-        <f t="shared" si="5"/>
-        <v>6830.8182500000003</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="1">
+        <f>B18+B19</f>
+        <v>7934.7104999999992</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" ref="C20:I20" si="8">C18+C19</f>
+        <v>7541.3583749999998</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="8"/>
+        <v>7338.2411250000005</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="8"/>
+        <v>7137.9872500000001</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="8"/>
+        <v>7048.9847499999996</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="8"/>
+        <v>6917.2090000000007</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="8"/>
+        <v>6872.0992500000011</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" si="8"/>
+        <v>6830.8182500000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="1">
-        <f>$B$19-B19</f>
+      <c r="B21" s="1">
+        <f>$B$20-B20</f>
         <v>0</v>
       </c>
-      <c r="C20" s="1">
-        <f t="shared" ref="C20:I20" si="6">$B$19-C19</f>
+      <c r="C21" s="1">
+        <f t="shared" ref="C21:I21" si="9">$B$20-C20</f>
         <v>393.35212499999943</v>
       </c>
-      <c r="D20" s="1">
-        <f t="shared" si="6"/>
+      <c r="D21" s="1">
+        <f t="shared" si="9"/>
         <v>596.46937499999876</v>
       </c>
-      <c r="E20" s="1">
-        <f t="shared" si="6"/>
+      <c r="E21" s="1">
+        <f t="shared" si="9"/>
         <v>796.7232499999991</v>
       </c>
-      <c r="F20" s="1">
-        <f t="shared" si="6"/>
+      <c r="F21" s="1">
+        <f t="shared" si="9"/>
         <v>885.72574999999961</v>
       </c>
-      <c r="G20" s="1">
-        <f t="shared" si="6"/>
+      <c r="G21" s="1">
+        <f t="shared" si="9"/>
         <v>1017.5014999999985</v>
       </c>
-      <c r="H20" s="1">
-        <f t="shared" si="6"/>
+      <c r="H21" s="1">
+        <f t="shared" si="9"/>
         <v>1062.6112499999981</v>
       </c>
-      <c r="I20" s="1">
-        <f t="shared" si="6"/>
+      <c r="I21" s="1">
+        <f t="shared" si="9"/>
         <v>1103.892249999999</v>
       </c>
     </row>

</xml_diff>